<commit_message>
Task ready for kid piloting
</commit_message>
<xml_diff>
--- a/pawStimuli.xlsx
+++ b/pawStimuli.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-31920" yWindow="3000" windowWidth="23920" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="1600" windowWidth="23920" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
   <si>
     <t>pawPatrol1</t>
   </si>
@@ -61,7 +61,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -104,8 +103,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -123,17 +124,19 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -502,6 +505,159 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>